<commit_message>
Fix 25: address issues handled
</commit_message>
<xml_diff>
--- a/25.ziplinesolutionsus/extracted_data/25.zipline.xlsx
+++ b/25.ziplinesolutionsus/extracted_data/25.zipline.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="98">
   <si>
     <t>name</t>
   </si>
@@ -71,12 +71,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Spencer-Valley-Ziplines.png</t>
   </si>
   <si>
+    <t>Redwood, New York</t>
+  </si>
+  <si>
     <t>(315) 767-3235</t>
   </si>
   <si>
-    <t>Redwood, New York</t>
-  </si>
-  <si>
     <t>Xtreme Park Adventures</t>
   </si>
   <si>
@@ -86,12 +86,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/XTreme-Park-Adventures-1.png</t>
   </si>
   <si>
+    <t>Durham, North Carolina</t>
+  </si>
+  <si>
     <t>(919) 596-6100</t>
   </si>
   <si>
-    <t>Durham, North Carolina</t>
-  </si>
-  <si>
     <t>The Children’s Movement Center</t>
   </si>
   <si>
@@ -101,12 +101,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Locations_300x200_ChildrensMovementCenter.jpg</t>
   </si>
   <si>
+    <t>New Milford, Connecticut</t>
+  </si>
+  <si>
     <t>(860) 799-6602</t>
   </si>
   <si>
-    <t>New Milford, Connecticut</t>
-  </si>
-  <si>
     <t>Soaring Cliffs</t>
   </si>
   <si>
@@ -152,12 +152,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/AdrenalineFallsZipline.jpg</t>
   </si>
   <si>
+    <t>Mackinaw City, Michigan</t>
+  </si>
+  <si>
     <t>(231) 436-5630</t>
   </si>
   <si>
-    <t>Mackinaw City, Michigan</t>
-  </si>
-  <si>
     <t>The Zone</t>
   </si>
   <si>
@@ -165,15 +165,15 @@
   </si>
   <si>
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Locations_300x200_TheZone.jpg</t>
-  </si>
-  <si>
-    <t>(732) 730-1002</t>
   </si>
   <si>
     <t>Gilboa, New York
 Stamford, New York</t>
   </si>
   <si>
+    <t>(732) 730-1002</t>
+  </si>
+  <si>
     <t>Riversport Adventures</t>
   </si>
   <si>
@@ -183,12 +183,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Locations_300x200_RiversportAdventures.jpg</t>
   </si>
   <si>
+    <t>Oklahoma City, Oklahoma</t>
+  </si>
+  <si>
     <t>(405) 552-4040</t>
   </si>
   <si>
-    <t>Oklahoma City, Oklahoma</t>
-  </si>
-  <si>
     <t>Holiday Mountain</t>
   </si>
   <si>
@@ -198,12 +198,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Holiday-Mountain-1.png</t>
   </si>
   <si>
+    <t>La Riviere, Manitoba, Canada</t>
+  </si>
+  <si>
     <t>(204) 242-2172</t>
   </si>
   <si>
-    <t>La Riviere, Manitoba, Canada</t>
-  </si>
-  <si>
     <t>Chuckster’s Family Fun Park</t>
   </si>
   <si>
@@ -213,12 +213,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Chucksters-Family-Fun-Park-Logo.jpg</t>
   </si>
   <si>
+    <t>Vestal, New York</t>
+  </si>
+  <si>
     <t>(607) 752-1070</t>
   </si>
   <si>
-    <t>Vestal, New York</t>
-  </si>
-  <si>
     <t>Rugaru Adventures</t>
   </si>
   <si>
@@ -228,12 +228,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Locations_300x200_RugaruAdventures.jpg</t>
   </si>
   <si>
+    <t>Broken Bow, Oklahoma</t>
+  </si>
+  <si>
     <t>(580) 494-2947</t>
   </si>
   <si>
-    <t>Broken Bow, Oklahoma</t>
-  </si>
-  <si>
     <t>Bounce – Abu Dhabi</t>
   </si>
   <si>
@@ -243,12 +243,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/12/Locations_300x200_Bounce.jpg</t>
   </si>
   <si>
+    <t>Al Marina, Abu Dhabi, United Arab Emirates</t>
+  </si>
+  <si>
     <t>+971 4 321 1400</t>
   </si>
   <si>
-    <t>Al Marina, Abu Dhabi, United Arab Emirates</t>
-  </si>
-  <si>
     <t>DropZone – Plymouth</t>
   </si>
   <si>
@@ -291,12 +291,12 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/11/Locations_300x200_BelmountPark.jpg</t>
   </si>
   <si>
+    <t>San Diego, California</t>
+  </si>
+  <si>
     <t>(858) 228-9283</t>
   </si>
   <si>
-    <t>San Diego, California</t>
-  </si>
-  <si>
     <t>Angry Birds Activity Park</t>
   </si>
   <si>
@@ -306,10 +306,10 @@
     <t>https://www.ziplinesolutionsus.com/wp-content/uploads/sites/4/2016/10/Locations_300x200_AngryBirdsActivityPark.jpg</t>
   </si>
   <si>
+    <t>St. Petersberg, Russia</t>
+  </si>
+  <si>
     <t>+7 (812) 602-06-67</t>
-  </si>
-  <si>
-    <t>St. Petersberg, Russia</t>
   </si>
 </sst>
 </file>
@@ -779,7 +779,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{d9a98710-f06f-4cd8-85d5-e0b4301f18d5}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2353308b-d56c-4a11-8b4d-976e97115906}">
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1"/>
@@ -789,7 +789,7 @@
     <col min="1" max="1" width="32.2857142857143" customWidth="1"/>
     <col min="2" max="2" width="75.7142857142857" customWidth="1"/>
     <col min="3" max="3" width="102.428571428571" customWidth="1"/>
-    <col min="4" max="4" width="23" customWidth="1"/>
+    <col min="4" max="4" width="37.7142857142857" customWidth="1"/>
     <col min="5" max="5" width="16.8571428571429" customWidth="1"/>
     <col min="6" max="6" width="13.5714285714286" customWidth="1"/>
     <col min="7" max="7" width="32.2857142857143" customWidth="1"/>
@@ -867,14 +867,17 @@
       <c r="C4" t="s">
         <v>17</v>
       </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
       <c r="E4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G4" t="s">
         <v>15</v>
       </c>
       <c r="H4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:8" s="4" customFormat="1" ht="12.75">
@@ -887,15 +890,17 @@
       <c r="C5" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>23</v>
+      </c>
       <c r="E5" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>20</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="12.75">
@@ -908,14 +913,17 @@
       <c r="C6" t="s">
         <v>27</v>
       </c>
+      <c r="D6" t="s">
+        <v>28</v>
+      </c>
       <c r="E6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G6" t="s">
         <v>25</v>
       </c>
       <c r="H6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="4" customFormat="1" ht="12.75">
@@ -974,15 +982,17 @@
       <c r="C9" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="4"/>
+      <c r="D9" s="4" t="s">
+        <v>45</v>
+      </c>
       <c r="E9" s="4" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>42</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="12.75">
@@ -995,17 +1005,20 @@
       <c r="C10" t="s">
         <v>49</v>
       </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
       <c r="E10" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G10" t="s">
         <v>47</v>
       </c>
       <c r="H10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="4" customFormat="1" ht="12.75">
@@ -1018,15 +1031,17 @@
       <c r="C11" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="D11" s="4"/>
+      <c r="D11" s="4" t="s">
+        <v>55</v>
+      </c>
       <c r="E11" s="4" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="12.75">
@@ -1039,14 +1054,17 @@
       <c r="C12" t="s">
         <v>59</v>
       </c>
+      <c r="D12" t="s">
+        <v>60</v>
+      </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G12" t="s">
         <v>57</v>
       </c>
       <c r="H12" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="4" customFormat="1" ht="12.75">
@@ -1059,15 +1077,17 @@
       <c r="C13" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="D13" s="4"/>
+      <c r="D13" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="E13" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>62</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="12.75">
@@ -1080,14 +1100,17 @@
       <c r="C14" t="s">
         <v>69</v>
       </c>
+      <c r="D14" t="s">
+        <v>70</v>
+      </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="G14" t="s">
         <v>67</v>
       </c>
       <c r="H14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:8" s="4" customFormat="1" ht="12.75">
@@ -1100,15 +1123,17 @@
       <c r="C15" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>75</v>
+      </c>
       <c r="E15" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="G15" s="4" t="s">
         <v>72</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="12.75">
@@ -1164,14 +1189,17 @@
       <c r="C18" t="s">
         <v>90</v>
       </c>
+      <c r="D18" t="s">
+        <v>91</v>
+      </c>
       <c r="E18" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="G18" t="s">
         <v>88</v>
       </c>
       <c r="H18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="4" customFormat="1" ht="12.75">
@@ -1184,15 +1212,17 @@
       <c r="C19" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="D19" s="4"/>
+      <c r="D19" s="4" t="s">
+        <v>96</v>
+      </c>
       <c r="E19" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>93</v>
       </c>
       <c r="H19" s="4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>